<commit_message>
mudancas para projeto maringa e londrina
</commit_message>
<xml_diff>
--- a/app_territory/data/regic/REGIC2018_Arranjos_Populacionais.xlsx
+++ b/app_territory/data/regic/REGIC2018_Arranjos_Populacionais.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sistema de inovacao\app_territory\data\regic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\innovation_panel\innovation_panel\app_territory\data\regic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9F1866-D3C8-4D53-99E4-E02509EB0691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D166E16-7DA1-429A-8C87-90CEC7707EEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Arranjos Populacionais'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Planilha1!$A$1:$F$961</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -20577,10 +20578,18 @@
   <dimension ref="A1:F961"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F961"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="89.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -37562,7 +37571,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F961" xr:uid="{B66E13C2-184B-4174-B47B-C7601E4237D3}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>